<commit_message>
some values changed, BOM added
</commit_message>
<xml_diff>
--- a/hardware/Datasheets/Berechnungen.xlsx
+++ b/hardware/Datasheets/Berechnungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\HFM_Adapter\hardware\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BA2ED9-FB68-46E0-91CF-D63012868AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10942CC-81ED-4D52-9286-032FD53C5ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D1B27DEE-E3C7-4633-8DAA-735C20D4774F}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="Temperatur" sheetId="3" r:id="rId3"/>
     <sheet name="ADC" sheetId="4" r:id="rId4"/>
     <sheet name="Spannungsteiler" sheetId="5" r:id="rId5"/>
-    <sheet name="TLE42764" sheetId="6" r:id="rId6"/>
+    <sheet name="OpAmp" sheetId="7" r:id="rId6"/>
+    <sheet name="TLE42764" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="36">
   <si>
     <t>Signature</t>
   </si>
@@ -276,6 +277,55 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>572005</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>86085</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E671C30-BCFA-88DE-7776-4A860AD2DEDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="361950"/>
+          <a:ext cx="3620005" cy="2581635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1907,11 +1957,11 @@
       </c>
       <c r="B15">
         <f>Spannungsteiler!B4</f>
-        <v>0.6470588235294118</v>
+        <v>0.66</v>
       </c>
       <c r="C15" s="4">
         <f>1/B15</f>
-        <v>1.5454545454545454</v>
+        <v>1.5151515151515151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,7 +1970,7 @@
       </c>
       <c r="B16">
         <f>B13*C15</f>
-        <v>4.5533935546874993</v>
+        <v>4.4641113281249991</v>
       </c>
     </row>
   </sheetData>
@@ -1933,7 +1983,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,10 +2005,10 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>6000</v>
+        <v>17000</v>
       </c>
       <c r="C2">
-        <v>18700</v>
+        <v>82000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1966,10 +2016,10 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>11000</v>
+        <v>33000</v>
       </c>
       <c r="C3">
-        <v>33000</v>
+        <v>10000</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -1984,18 +2034,18 @@
       </c>
       <c r="B4">
         <f>B3/(B2+B3)</f>
-        <v>0.6470588235294118</v>
+        <v>0.66</v>
       </c>
       <c r="C4">
         <f>C3/(C2+C3)</f>
-        <v>0.63829787234042556</v>
+        <v>0.10869565217391304</v>
       </c>
       <c r="I4" s="3">
         <v>4.4569999999999999</v>
       </c>
       <c r="J4" s="3">
         <f>I4*$B$4</f>
-        <v>2.8839411764705885</v>
+        <v>2.9416199999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2004,18 +2054,18 @@
       </c>
       <c r="B5">
         <f>B1*B4</f>
-        <v>3.2352941176470589</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="C5">
         <f>B1*C4</f>
-        <v>3.1914893617021276</v>
+        <v>0.54347826086956519</v>
       </c>
       <c r="I5" s="3">
         <v>4.1689999999999996</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J7" si="0">I5*$B$4</f>
-        <v>2.6975882352941176</v>
+        <v>2.7515399999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2024,20 +2074,20 @@
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>2.4258235294117649</v>
+        <v>2.4743400000000002</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>1/B4</f>
-        <v>1.5454545454545454</v>
+        <v>1.5151515151515151</v>
       </c>
       <c r="I7" s="3">
         <v>2.9990000000000001</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>1.9405294117647061</v>
+        <v>1.9793400000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2047,11 +2097,69 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49090171-3C73-4133-A5B8-200475357F02}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <f>1+(B3/B2)</f>
+        <v>1.5151515151515151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>B1*B4</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7369C0AA-89AE-403A-BD11-4EBDFA2B0A24}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
some changed rev 1.0
</commit_message>
<xml_diff>
--- a/hardware/Datasheets/Berechnungen.xlsx
+++ b/hardware/Datasheets/Berechnungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\HFM_Adapter\hardware\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10942CC-81ED-4D52-9286-032FD53C5ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33F824B-AFE8-44E2-9043-FC03ABB7539A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D1B27DEE-E3C7-4633-8DAA-735C20D4774F}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{D1B27DEE-E3C7-4633-8DAA-735C20D4774F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1982,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D67C15F-E165-4476-B43D-6E820F3A7FAB}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,7 +2008,7 @@
         <v>17000</v>
       </c>
       <c r="C2">
-        <v>82000</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C4">
         <f>C3/(C2+C3)</f>
-        <v>0.10869565217391304</v>
+        <v>0.64102564102564108</v>
       </c>
       <c r="I4" s="3">
         <v>4.4569999999999999</v>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="C5">
         <f>B1*C4</f>
-        <v>0.54347826086956519</v>
+        <v>3.2051282051282053</v>
       </c>
       <c r="I5" s="3">
         <v>4.1689999999999996</v>
@@ -2100,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49090171-3C73-4133-A5B8-200475357F02}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2119,7 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>33000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>17000</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="B4">
         <f>1+(B3/B2)</f>
-        <v>1.5151515151515151</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B5">
         <f>B1*B4</f>
-        <v>5</v>
+        <v>5.1479999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>